<commit_message>
hope everything is okay
</commit_message>
<xml_diff>
--- a/Potential MSRI participants.xlsx
+++ b/Potential MSRI participants.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="42660" yWindow="2620" windowWidth="39700" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="32000" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Potential MSRI participants" sheetId="1" r:id="rId1"/>
     <sheet name="Statistics" sheetId="2" r:id="rId2"/>
     <sheet name="Declined" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1770,7 +1770,7 @@
   </sheetPr>
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4683,7 +4683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final update for the proposal: Chelsea
</commit_message>
<xml_diff>
--- a/Potential MSRI participants.xlsx
+++ b/Potential MSRI participants.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Potential MSRI participants" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="460">
   <si>
     <t>Country</t>
   </si>
@@ -1382,9 +1382,6 @@
   </si>
   <si>
     <t>possibly entire semester; also involved in the companion workship</t>
-  </si>
-  <si>
-    <t>whole semester</t>
   </si>
   <si>
     <t>more than a month</t>
@@ -1770,11 +1767,11 @@
   </sheetPr>
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1809,7 +1806,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -1818,7 +1815,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>3</v>
@@ -1943,7 +1940,7 @@
         <v>179</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E5" t="s">
         <v>259</v>
@@ -2022,53 +2019,65 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>415</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s">
-        <v>416</v>
+        <v>338</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>419</v>
+        <v>179</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="E8" t="s">
+        <v>340</v>
       </c>
       <c r="F8" t="s">
-        <v>418</v>
+        <v>339</v>
       </c>
       <c r="G8" t="s">
-        <v>417</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s">
         <v>67</v>
       </c>
       <c r="K8" s="9">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="B9" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="C9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>432</v>
+      <c r="E9" s="5" t="s">
+        <v>419</v>
       </c>
       <c r="F9" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="G9" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="H9" t="s">
         <v>29</v>
@@ -2076,55 +2085,55 @@
       <c r="J9" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="L9" s="1"/>
+      <c r="K9" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>357</v>
+        <v>428</v>
       </c>
       <c r="B10" t="s">
-        <v>358</v>
+        <v>429</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>377</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>440</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J10" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>143</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>357</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>358</v>
       </c>
       <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="E11" t="s">
-        <v>68</v>
+      <c r="E11" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>459</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
@@ -2136,21 +2145,21 @@
         <v>67</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
         <v>64</v>
@@ -2159,124 +2168,118 @@
         <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
         <v>67</v>
       </c>
-      <c r="K12" s="9">
-        <v>1</v>
+      <c r="K12" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>363</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>364</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>379</v>
+      <c r="E13" t="s">
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>229</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J13" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="9" t="s">
-        <v>243</v>
+      <c r="K13" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>430</v>
+        <v>363</v>
       </c>
       <c r="B14" t="s">
-        <v>422</v>
+        <v>364</v>
       </c>
       <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>431</v>
+      <c r="E14" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="F14" t="s">
-        <v>441</v>
+        <v>229</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
         <v>67</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>430</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>422</v>
       </c>
       <c r="C15" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
-        <v>182</v>
+      <c r="E15" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="F15" t="s">
-        <v>229</v>
+        <v>441</v>
       </c>
       <c r="G15" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J15" t="s">
         <v>67</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="L15" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>370</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>371</v>
+        <v>177</v>
       </c>
       <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>376</v>
+      <c r="E16" t="s">
+        <v>182</v>
       </c>
       <c r="F16" t="s">
-        <v>372</v>
+        <v>229</v>
       </c>
       <c r="G16" t="s">
         <v>142</v>
@@ -2287,60 +2290,66 @@
       <c r="J16" t="s">
         <v>67</v>
       </c>
-      <c r="K16" s="9">
-        <v>5</v>
+      <c r="K16" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="L16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>370</v>
       </c>
       <c r="B17" t="s">
-        <v>274</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="E17" t="s">
-        <v>276</v>
+      <c r="E17" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="F17" t="s">
-        <v>275</v>
+        <v>372</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="J17" t="s">
         <v>67</v>
       </c>
       <c r="K17" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>273</v>
       </c>
       <c r="B18" t="s">
-        <v>320</v>
+        <v>274</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="F18" t="s">
-        <v>148</v>
+        <v>275</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J18" t="s">
         <v>67</v>
@@ -2351,19 +2360,19 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>322</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C19" t="s">
         <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F19" t="s">
-        <v>324</v>
+        <v>148</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -2380,19 +2389,19 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>359</v>
+        <v>322</v>
       </c>
       <c r="B20" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="C20" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>378</v>
+      <c r="E20" t="s">
+        <v>325</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>324</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
@@ -2404,53 +2413,50 @@
         <v>67</v>
       </c>
       <c r="K20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>359</v>
+      </c>
+      <c r="B21" t="s">
+        <v>360</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" s="9">
         <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="64" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="9">
-        <v>3</v>
-      </c>
-      <c r="L21" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
@@ -2468,146 +2474,152 @@
         <v>42318</v>
       </c>
       <c r="M22" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="9">
+        <v>3</v>
+      </c>
+      <c r="L23" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>23</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>21</v>
       </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" s="9">
-        <v>5</v>
-      </c>
-      <c r="L23" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" t="s">
-        <v>27</v>
-      </c>
       <c r="G24" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H24" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="K24" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="L24" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E26" t="s">
         <v>34</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>32</v>
       </c>
-      <c r="G25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="9" t="s">
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L26" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="1">
-        <v>42318</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>365</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>367</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>374</v>
+      <c r="E27" t="s">
+        <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>373</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -2615,619 +2627,619 @@
       <c r="H27" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="9">
-        <v>2</v>
+      <c r="L27" s="1">
+        <v>42318</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>365</v>
+      </c>
+      <c r="B28" t="s">
+        <v>367</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F28" t="s">
+        <v>373</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>368</v>
       </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>86</v>
       </c>
-      <c r="G28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="9" t="s">
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>48</v>
       </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
         <v>51</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>49</v>
       </c>
-      <c r="G29" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" t="s">
-        <v>29</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L29" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>424</v>
-      </c>
-      <c r="B30" t="s">
-        <v>423</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="F30" t="s">
-        <v>160</v>
-      </c>
       <c r="G30" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="H30" t="s">
         <v>29</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="L30" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="L30" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="B31" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="F31" t="s">
-        <v>413</v>
+        <v>160</v>
       </c>
       <c r="G31" t="s">
-        <v>22</v>
+        <v>161</v>
       </c>
       <c r="H31" t="s">
         <v>29</v>
       </c>
-      <c r="K31" s="9">
+      <c r="K31" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B32" t="s">
+        <v>411</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="F32" t="s">
+        <v>413</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" t="s">
+        <v>29</v>
+      </c>
+      <c r="K32" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="80" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>54</v>
       </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
         <v>56</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>55</v>
       </c>
-      <c r="G32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" s="9">
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="9">
         <v>5</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" t="s">
-        <v>60</v>
-      </c>
-      <c r="G33" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="9">
-        <v>8</v>
-      </c>
-      <c r="L33" s="1">
-        <v>42318</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>408</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>409</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>414</v>
+      <c r="E34" t="s">
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>366</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="H34" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="K34" s="9">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="L34" s="1">
+        <v>42318</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="B35" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="F35" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="H35" t="s">
         <v>29</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>403</v>
+      </c>
+      <c r="B36" t="s">
+        <v>404</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F36" t="s">
+        <v>405</v>
+      </c>
+      <c r="G36" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" t="s">
+        <v>29</v>
+      </c>
+      <c r="K36" s="9" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>69</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
         <v>73</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>71</v>
       </c>
-      <c r="G36" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" s="9" t="s">
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="L36" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M36" s="3" t="s">
+      <c r="L37" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M37" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>84</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>85</v>
       </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
         <v>87</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>86</v>
       </c>
-      <c r="G37" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" s="9">
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="9">
         <v>1</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L38" t="s">
         <v>35</v>
       </c>
-      <c r="M37" s="3" t="s">
+      <c r="M38" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>89</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>90</v>
       </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>91</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>39</v>
       </c>
-      <c r="G38" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="G39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" t="s">
         <v>29</v>
       </c>
-      <c r="K38" s="9">
+      <c r="K39" s="9">
         <v>8</v>
       </c>
-      <c r="L38" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M38" s="3" t="s">
+      <c r="L39" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M39" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="N38" s="3" t="s">
+      <c r="N39" s="3" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>97</v>
       </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
         <v>99</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>98</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>81</v>
       </c>
-      <c r="H39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" s="9">
+      <c r="H40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="9">
         <v>4</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L40" t="s">
         <v>35</v>
       </c>
-      <c r="M39" s="3" t="s">
+      <c r="M40" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>427</v>
-      </c>
-      <c r="B40" t="s">
-        <v>421</v>
-      </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="F40" t="s">
-        <v>436</v>
-      </c>
-      <c r="G40" t="s">
-        <v>437</v>
-      </c>
-      <c r="H40" t="s">
-        <v>29</v>
-      </c>
-      <c r="K40" s="9">
-        <v>3</v>
-      </c>
-      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>427</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>421</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
       </c>
-      <c r="E41" t="s">
-        <v>105</v>
+      <c r="E41" s="2" t="s">
+        <v>435</v>
       </c>
       <c r="F41" t="s">
-        <v>103</v>
+        <v>436</v>
       </c>
       <c r="G41" t="s">
-        <v>104</v>
+        <v>437</v>
       </c>
       <c r="H41" t="s">
-        <v>13</v>
-      </c>
-      <c r="L41" s="1">
-        <v>42318</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="K41" s="9">
+        <v>3</v>
+      </c>
+      <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H42" t="s">
+        <v>13</v>
+      </c>
+      <c r="L42" s="1">
+        <v>42318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>106</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>107</v>
       </c>
-      <c r="C42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
         <v>109</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>108</v>
       </c>
-      <c r="G42" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" s="9">
+      <c r="G43" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="9">
         <v>5</v>
       </c>
-      <c r="L42" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M42" s="3" t="s">
+      <c r="L43" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M43" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="64" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>120</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="C43" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
         <v>124</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>122</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>123</v>
       </c>
-      <c r="H43" t="s">
-        <v>13</v>
-      </c>
-      <c r="K43" s="9" t="s">
+      <c r="H44" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L43" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M43" s="3" t="s">
+      <c r="L44" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M44" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>126</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>127</v>
       </c>
-      <c r="C44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
         <v>131</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>128</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
         <v>129</v>
       </c>
-      <c r="H44" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="9" t="s">
+      <c r="H45" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="L44" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M44" s="3" t="s">
+      <c r="L45" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M45" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>133</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>134</v>
       </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
         <v>137</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>135</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G46" t="s">
         <v>136</v>
       </c>
-      <c r="H45" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" s="9" t="s">
+      <c r="H46" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="L45" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M45" s="3" t="s">
+      <c r="L46" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M46" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="64" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>139</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>140</v>
       </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
         <v>144</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>141</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>142</v>
       </c>
-      <c r="H46" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" s="9" t="s">
+      <c r="H47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="L46" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M46" s="3" t="s">
+      <c r="L47" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M47" s="3" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47" t="s">
-        <v>147</v>
-      </c>
-      <c r="C47" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" t="s">
-        <v>149</v>
-      </c>
-      <c r="F47" t="s">
-        <v>148</v>
-      </c>
-      <c r="G47" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" t="s">
-        <v>13</v>
-      </c>
-      <c r="K47" s="9">
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B48" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C48" t="s">
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F48" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="G48" t="s">
         <v>22</v>
@@ -3236,347 +3248,344 @@
         <v>13</v>
       </c>
       <c r="K48" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>153</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>154</v>
       </c>
-      <c r="C49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
         <v>157</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>155</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>156</v>
       </c>
-      <c r="H49" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" s="9">
+      <c r="H50" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" s="9">
         <v>3</v>
       </c>
-      <c r="L49" s="1">
-        <v>42318</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="L50" s="1">
+        <v>42318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>158</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>159</v>
       </c>
-      <c r="C50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" t="s">
         <v>163</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>160</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" t="s">
         <v>161</v>
       </c>
-      <c r="H50" t="s">
-        <v>13</v>
-      </c>
-      <c r="K50" s="9" t="s">
+      <c r="H51" t="s">
+        <v>13</v>
+      </c>
+      <c r="K51" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="L50" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M50" s="3" t="s">
+      <c r="L51" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M51" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="N50" s="3" t="s">
+      <c r="N51" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>171</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>172</v>
       </c>
-      <c r="C51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
         <v>174</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>108</v>
       </c>
-      <c r="G51" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" t="s">
-        <v>13</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="G52" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" t="s">
         <v>67</v>
       </c>
-      <c r="K51" s="9" t="s">
+      <c r="K52" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="L51" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M51" s="3" t="s">
+      <c r="L52" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M52" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="64" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>19</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>184</v>
       </c>
-      <c r="C52" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>186</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>185</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>81</v>
       </c>
-      <c r="H52" t="s">
-        <v>13</v>
-      </c>
-      <c r="K52" s="9" t="s">
+      <c r="H53" t="s">
+        <v>13</v>
+      </c>
+      <c r="K53" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="L52" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M52" s="3" t="s">
+      <c r="L53" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M53" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="N52" s="3" t="s">
+      <c r="N53" s="3" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>188</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>189</v>
       </c>
-      <c r="C53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" t="s">
         <v>191</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>190</v>
       </c>
-      <c r="G53" t="s">
-        <v>22</v>
-      </c>
-      <c r="H53" t="s">
-        <v>13</v>
-      </c>
-      <c r="K53" s="9" t="s">
+      <c r="G54" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" t="s">
+        <v>13</v>
+      </c>
+      <c r="K54" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="L53" s="1">
-        <v>42318</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>192</v>
-      </c>
-      <c r="B54" t="s">
-        <v>193</v>
-      </c>
-      <c r="C54" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="E54" t="s">
-        <v>196</v>
-      </c>
-      <c r="F54" t="s">
-        <v>194</v>
-      </c>
-      <c r="G54" t="s">
-        <v>168</v>
-      </c>
-      <c r="H54" t="s">
-        <v>13</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="L54" s="1">
         <v>42318</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="N54" s="3" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E55" t="s">
+        <v>196</v>
+      </c>
+      <c r="F55" t="s">
+        <v>194</v>
+      </c>
+      <c r="G55" t="s">
+        <v>168</v>
+      </c>
+      <c r="H55" t="s">
+        <v>13</v>
+      </c>
+      <c r="K55" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="L55" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>198</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>199</v>
       </c>
-      <c r="C55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" t="s">
         <v>201</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F56" t="s">
         <v>200</v>
       </c>
-      <c r="G55" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" t="s">
-        <v>13</v>
-      </c>
-      <c r="K55" s="9">
+      <c r="G56" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" t="s">
+        <v>13</v>
+      </c>
+      <c r="K56" s="9">
         <v>5</v>
       </c>
-      <c r="L55" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M55" s="3" t="s">
+      <c r="L56" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M56" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>69</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>203</v>
       </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s">
         <v>204</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" t="s">
         <v>190</v>
       </c>
-      <c r="G56" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" t="s">
-        <v>13</v>
-      </c>
-      <c r="K56" s="9" t="s">
+      <c r="G57" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" t="s">
+        <v>13</v>
+      </c>
+      <c r="K57" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="64" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>205</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>206</v>
       </c>
-      <c r="C57" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>209</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F58" t="s">
         <v>207</v>
       </c>
-      <c r="G57" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" t="s">
-        <v>13</v>
-      </c>
-      <c r="K57" s="9" t="s">
+      <c r="G58" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" t="s">
+        <v>13</v>
+      </c>
+      <c r="K58" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="L57" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M57" s="4" t="s">
+      <c r="L58" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M58" s="4" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" t="s">
-        <v>211</v>
-      </c>
-      <c r="C58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>213</v>
-      </c>
-      <c r="F58" t="s">
-        <v>212</v>
-      </c>
-      <c r="G58" t="s">
-        <v>22</v>
-      </c>
-      <c r="H58" t="s">
-        <v>13</v>
-      </c>
-      <c r="K58" s="9">
-        <v>7</v>
-      </c>
-      <c r="L58" s="1">
-        <v>42318</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F59" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G59" t="s">
         <v>22</v>
@@ -3584,290 +3593,284 @@
       <c r="H59" t="s">
         <v>13</v>
       </c>
-      <c r="J59" t="s">
-        <v>67</v>
-      </c>
-      <c r="K59" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="L59" t="s">
-        <v>35</v>
-      </c>
-      <c r="M59" s="3" t="s">
-        <v>219</v>
+      <c r="K59" s="9">
+        <v>7</v>
+      </c>
+      <c r="L59" s="1">
+        <v>42318</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C60" t="s">
         <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F60" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G60" t="s">
         <v>22</v>
       </c>
       <c r="H60" t="s">
         <v>13</v>
+      </c>
+      <c r="J60" t="s">
+        <v>67</v>
+      </c>
+      <c r="K60" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="L60" t="s">
+        <v>35</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>220</v>
+      </c>
+      <c r="B61" t="s">
+        <v>221</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>223</v>
+      </c>
+      <c r="F61" t="s">
+        <v>222</v>
+      </c>
+      <c r="G61" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>224</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>225</v>
       </c>
-      <c r="C61" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
         <v>226</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F62" t="s">
         <v>216</v>
       </c>
-      <c r="G61" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" t="s">
-        <v>13</v>
-      </c>
-      <c r="K61" s="9">
+      <c r="G62" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" t="s">
+        <v>13</v>
+      </c>
+      <c r="K62" s="9">
         <v>5</v>
       </c>
-      <c r="L61" s="1">
-        <v>42318</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="L62" s="1">
+        <v>42318</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>116</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>362</v>
       </c>
-      <c r="C62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s">
         <v>234</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>232</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G63" t="s">
         <v>161</v>
       </c>
-      <c r="H62" t="s">
-        <v>13</v>
-      </c>
-      <c r="K62" s="9" t="s">
+      <c r="H63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K63" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="L62" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M62" s="3" t="s">
+      <c r="L63" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M63" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="64" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>236</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>237</v>
       </c>
-      <c r="C63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s">
         <v>238</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>10</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G64" t="s">
         <v>11</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H64" t="s">
         <v>29</v>
       </c>
-      <c r="K63" s="9">
+      <c r="K64" s="9">
         <v>3</v>
       </c>
-      <c r="L63" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M63" s="3" t="s">
+      <c r="L64" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M64" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>240</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>241</v>
       </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" t="s">
         <v>244</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>242</v>
       </c>
-      <c r="G64" t="s">
-        <v>22</v>
-      </c>
-      <c r="H64" t="s">
-        <v>13</v>
-      </c>
-      <c r="K64" s="9" t="s">
+      <c r="G65" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" t="s">
+        <v>13</v>
+      </c>
+      <c r="K65" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="80" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="66" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>245</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>246</v>
       </c>
-      <c r="C65" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="3" t="s">
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="E66" t="s">
+        <v>248</v>
+      </c>
+      <c r="F66" t="s">
+        <v>247</v>
+      </c>
+      <c r="G66" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" t="s">
+        <v>13</v>
+      </c>
+      <c r="K66" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="L66" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M66" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="N66" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="E65" t="s">
-        <v>248</v>
-      </c>
-      <c r="F65" t="s">
-        <v>247</v>
-      </c>
-      <c r="G65" t="s">
-        <v>22</v>
-      </c>
-      <c r="H65" t="s">
-        <v>13</v>
-      </c>
-      <c r="K65" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L65" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M65" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="N65" s="3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" t="s">
-        <v>253</v>
-      </c>
-      <c r="C66" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>254</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F67" t="s">
         <v>369</v>
       </c>
-      <c r="G66" t="s">
-        <v>22</v>
-      </c>
-      <c r="H66" t="s">
-        <v>13</v>
-      </c>
-      <c r="K66" s="9" t="s">
+      <c r="G67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" t="s">
+        <v>13</v>
+      </c>
+      <c r="K67" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="L66" t="s">
+      <c r="L67" t="s">
         <v>35</v>
       </c>
-      <c r="M66" s="3" t="s">
+      <c r="M67" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="N66" s="3" t="s">
+      <c r="N67" s="3" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="80" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>260</v>
-      </c>
-      <c r="B67" t="s">
-        <v>261</v>
-      </c>
-      <c r="C67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E67" t="s">
-        <v>263</v>
-      </c>
-      <c r="F67" t="s">
-        <v>55</v>
-      </c>
-      <c r="G67" t="s">
-        <v>22</v>
-      </c>
-      <c r="H67" t="s">
-        <v>29</v>
-      </c>
-      <c r="K67" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="L67" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M67" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="N67" s="3" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>260</v>
       </c>
       <c r="B68" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C68" t="s">
         <v>12</v>
       </c>
+      <c r="D68" s="3" t="s">
+        <v>446</v>
+      </c>
       <c r="E68" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F68" t="s">
-        <v>265</v>
+        <v>55</v>
       </c>
       <c r="G68" t="s">
         <v>22</v>
@@ -3875,40 +3878,43 @@
       <c r="H68" t="s">
         <v>29</v>
       </c>
-      <c r="J68" t="s">
+      <c r="K68" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="L68" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>260</v>
+      </c>
+      <c r="B69" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" t="s">
+        <v>266</v>
+      </c>
+      <c r="F69" t="s">
+        <v>265</v>
+      </c>
+      <c r="G69" t="s">
+        <v>22</v>
+      </c>
+      <c r="H69" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" t="s">
         <v>67</v>
-      </c>
-      <c r="K68" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="L68" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M68" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>281</v>
-      </c>
-      <c r="B69" t="s">
-        <v>282</v>
-      </c>
-      <c r="C69" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" t="s">
-        <v>284</v>
-      </c>
-      <c r="F69" t="s">
-        <v>283</v>
-      </c>
-      <c r="G69" t="s">
-        <v>156</v>
-      </c>
-      <c r="H69" t="s">
-        <v>13</v>
       </c>
       <c r="K69" s="9" t="s">
         <v>243</v>
@@ -3916,60 +3922,54 @@
       <c r="L69" s="1">
         <v>42318</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+      <c r="M69" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B70" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>448</v>
-      </c>
       <c r="E70" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F70" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G70" t="s">
         <v>156</v>
       </c>
       <c r="H70" t="s">
-        <v>29</v>
-      </c>
-      <c r="J70" t="s">
-        <v>67</v>
-      </c>
-      <c r="K70" s="9">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="K70" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="L70" s="1">
         <v>42318</v>
       </c>
-      <c r="M70" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="N70" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>285</v>
       </c>
       <c r="B71" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C71" t="s">
         <v>12</v>
       </c>
+      <c r="D71" s="3" t="s">
+        <v>448</v>
+      </c>
       <c r="E71" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F71" t="s">
         <v>287</v>
@@ -3978,30 +3978,39 @@
         <v>156</v>
       </c>
       <c r="H71" t="s">
-        <v>13</v>
-      </c>
-      <c r="K71" s="9" t="s">
-        <v>65</v>
+        <v>29</v>
+      </c>
+      <c r="J71" t="s">
+        <v>67</v>
+      </c>
+      <c r="K71" s="9">
+        <v>5</v>
       </c>
       <c r="L71" s="1">
         <v>42318</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M71" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="N71" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>293</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
       </c>
       <c r="E72" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F72" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G72" t="s">
         <v>156</v>
@@ -4010,68 +4019,68 @@
         <v>13</v>
       </c>
       <c r="K72" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L72" s="1">
+        <v>42318</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>293</v>
+      </c>
+      <c r="B73" t="s">
+        <v>294</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" t="s">
+        <v>296</v>
+      </c>
+      <c r="F73" t="s">
+        <v>295</v>
+      </c>
+      <c r="G73" t="s">
+        <v>156</v>
+      </c>
+      <c r="H73" t="s">
+        <v>13</v>
+      </c>
+      <c r="K73" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L72" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M72" s="3" t="s">
+      <c r="L73" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M73" s="3" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>298</v>
-      </c>
-      <c r="B73" t="s">
-        <v>299</v>
-      </c>
-      <c r="C73" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" t="s">
-        <v>300</v>
-      </c>
-      <c r="F73" t="s">
-        <v>270</v>
-      </c>
-      <c r="G73" t="s">
-        <v>22</v>
-      </c>
-      <c r="H73" t="s">
-        <v>29</v>
-      </c>
-      <c r="K73" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="L73" s="1">
-        <v>42318</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B74" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F74" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="G74" t="s">
         <v>22</v>
       </c>
       <c r="H74" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>33</v>
+        <v>243</v>
       </c>
       <c r="L74" s="1">
         <v>42318</v>
@@ -4079,80 +4088,80 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B75" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C75" t="s">
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F75" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G75" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="H75" t="s">
-        <v>29</v>
-      </c>
-      <c r="K75" s="9">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="K75" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L75" s="1">
+        <v>42318</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B76" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="C76" t="s">
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="F76" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="G76" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="H76" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="K76" s="9">
         <v>5</v>
       </c>
-      <c r="L76" s="1">
-        <v>42318</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B77" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F77" t="s">
-        <v>207</v>
+        <v>303</v>
       </c>
       <c r="G77" t="s">
         <v>22</v>
       </c>
       <c r="H77" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="K77" s="9">
         <v>5</v>
@@ -4160,81 +4169,69 @@
       <c r="L77" s="1">
         <v>42318</v>
       </c>
-      <c r="M77" s="4" t="s">
+    </row>
+    <row r="78" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>329</v>
+      </c>
+      <c r="B78" t="s">
+        <v>330</v>
+      </c>
+      <c r="C78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>331</v>
+      </c>
+      <c r="F78" t="s">
+        <v>207</v>
+      </c>
+      <c r="G78" t="s">
+        <v>22</v>
+      </c>
+      <c r="H78" t="s">
+        <v>29</v>
+      </c>
+      <c r="K78" s="9">
+        <v>5</v>
+      </c>
+      <c r="L78" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M78" s="4" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>333</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>334</v>
       </c>
-      <c r="C78" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s">
         <v>335</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F79" t="s">
         <v>118</v>
       </c>
-      <c r="G78" t="s">
-        <v>22</v>
-      </c>
-      <c r="H78" t="s">
-        <v>13</v>
-      </c>
-      <c r="K78" s="9" t="s">
+      <c r="G79" t="s">
+        <v>22</v>
+      </c>
+      <c r="H79" t="s">
+        <v>13</v>
+      </c>
+      <c r="K79" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="L78" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M78" s="3" t="s">
+      <c r="L79" s="1">
+        <v>42318</v>
+      </c>
+      <c r="M79" s="3" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>337</v>
-      </c>
-      <c r="B79" t="s">
-        <v>338</v>
-      </c>
-      <c r="C79" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="E79" t="s">
-        <v>340</v>
-      </c>
-      <c r="F79" t="s">
-        <v>339</v>
-      </c>
-      <c r="G79" t="s">
-        <v>22</v>
-      </c>
-      <c r="H79" t="s">
-        <v>29</v>
-      </c>
-      <c r="I79" t="s">
-        <v>67</v>
-      </c>
-      <c r="K79" s="9">
-        <v>3</v>
-      </c>
-      <c r="L79" s="1">
-        <v>42318</v>
-      </c>
-      <c r="M79" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="N79" s="3" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4338,7 +4335,7 @@
         <v>44</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E83" t="s">
         <v>45</v>
@@ -4498,7 +4495,7 @@
         <v>44</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E88" t="s">
         <v>169</v>
@@ -4595,7 +4592,7 @@
         <v>44</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E91" t="s">
         <v>318</v>
@@ -4660,20 +4657,20 @@
     <sortCondition ref="B2:B92"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1"/>
-    <hyperlink ref="E28" r:id="rId2"/>
-    <hyperlink ref="E16" r:id="rId3"/>
-    <hyperlink ref="E10" r:id="rId4"/>
-    <hyperlink ref="E20" r:id="rId5"/>
-    <hyperlink ref="E13" r:id="rId6"/>
-    <hyperlink ref="E35" r:id="rId7"/>
-    <hyperlink ref="E31" r:id="rId8"/>
-    <hyperlink ref="E34" r:id="rId9"/>
-    <hyperlink ref="E8" r:id="rId10"/>
-    <hyperlink ref="E9" r:id="rId11"/>
-    <hyperlink ref="E30" r:id="rId12"/>
-    <hyperlink ref="E40" r:id="rId13"/>
-    <hyperlink ref="E14" r:id="rId14"/>
+    <hyperlink ref="E28" r:id="rId1"/>
+    <hyperlink ref="E29" r:id="rId2"/>
+    <hyperlink ref="E17" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId4"/>
+    <hyperlink ref="E21" r:id="rId5"/>
+    <hyperlink ref="E14" r:id="rId6"/>
+    <hyperlink ref="E36" r:id="rId7"/>
+    <hyperlink ref="E32" r:id="rId8"/>
+    <hyperlink ref="E35" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E31" r:id="rId12"/>
+    <hyperlink ref="E41" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4683,7 +4680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>